<commit_message>
added in/out adjacency list for network flow
</commit_message>
<xml_diff>
--- a/pickle/spd16_ships3_days15_methodGEN_schedules10.pkl.xlsx
+++ b/pickle/spd16_ships3_days15_methodGEN_schedules10.pkl.xlsx
@@ -386,170 +386,170 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['r3', 'r3', 'rTransit', 'r9', 'rTransit', 'r11', 'rTransit', 'r8', 'rTransit', 'r10', 'r12', 'rTransit', 'r9', 'rTransit', 'r12']</t>
+          <t>['rTransit', 'r8', 'rTransit', 'r4', 'r7', 'r4', 'rTransit', 'r8', 'r9', 'rTransit', 'r2', 'r4', 'rTransit', 'rTransit', 'r11']</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r2', 'rTransit', 'r10', 'r9', 'rTransit', 'r2', 'rTransit', 'r10', 'rTransit', 'r7', 'rTransit', 'r12', 'r10']</t>
+          <t>['rTransit', 'r8', 'rTransit', 'r7', 'rTransit', 'r5', 'r8', 'r9', 'r9', 'rTransit', 'r3', 'rTransit', 'r9', 'r9', 'r10']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r5', 'rTransit', 'r9', 'rTransit', 'r11', 'rTransit', 'r9', 'rTransit', 'r5', 'r3', 'r2']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r12', 'rTransit', 'r8', 'r5', 'rTransit', 'r9', 'rTransit', 'r12', 'rTransit', 'r5', 'r4']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>['r7', 'rTransit', 'r8', 'r8', 'rTransit', 'r12', 'rTransit', 'r8', 'r9', 'r8', 'rTransit', 'r7', 'rTransit', 'rTransit', 'r13']</t>
+          <t>['r4', 'r2', 'r4', 'rTransit', 'r9', 'rTransit', 'r7', 'rTransit', 'rTransit', 'r13', 'rTransit', 'r10', 'rTransit', 'r8', 'r9']</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['r13', 'rTransit', 'rTransit', 'r3', 'rTransit', 'r8', 'r9', 'rTransit', 'r4', 'rTransit', 'r10', 'rTransit', 'r8', 'r5', 'r4']</t>
+          <t>['rTransit', 'r10', 'rTransit', 'r8', 'r8', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r13', 'rTransit', 'r9', 'rTransit', 'r12', 'r11']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r5', 'rTransit', 'r9', 'rTransit', 'r4', 'r4', 'r2']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r10', 'rTransit', 'r8', 'rTransit', 'r11', 'rTransit', 'r8', 'rTransit', 'r2', 'rTransit', 'r9']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r13', 'rTransit', 'r12', 'rTransit', 'r3', 'r3', 'rTransit', 'r11', 'rTransit', 'r9', 'r10', 'r9', 'r8']</t>
+          <t>['rTransit', 'r10', 'rTransit', 'r2', 'rTransit', 'r10', 'r9', 'rTransit', 'r3', 'rTransit', 'r12', 'rTransit', 'r13', 'rTransit', 'r8']</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r7', 'rTransit', 'r9', 'rTransit', 'r5', 'rTransit', 'r12', 'r12', 'rTransit', 'r5', 'rTransit', 'r10', 'r10']</t>
+          <t>['rTransit', 'r8', 'rTransit', 'r3', 'rTransit', 'r9', 'r10', 'r10', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r7', 'r7', 'r7']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r10', 'rTransit', 'r4', 'r2', 'rTransit', 'r12', 'rTransit', 'r9', 'rTransit', 'r3', 'r4']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'rTransit', 'r11', 'rTransit', 'r3', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r2', 'rTransit', 'r10']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>['rTransit', 'r8', 'rTransit', 'r1', 'r3', 'r2', 'rTransit', 'r10', 'r9', 'rTransit', 'r12', 'rTransit', 'r13', 'rTransit', 'r9']</t>
+          <t>['rTransit', 'r10', 'rTransit', 'r11', 'rTransit', 'r3', 'rTransit', 'r10', 'r10', 'rTransit', 'r4', 'rTransit', 'r9', 'r8', 'r5']</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r4', 'r5', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r7', 'rTransit', 'r9', 'rTransit', 'r2', 'rTransit', 'r9']</t>
+          <t>['r11', 'rTransit', 'r10', 'rTransit', 'r3', 'rTransit', 'r12', 'rTransit', 'r7', 'rTransit', 'r8', 'r9', 'rTransit', 'r11', 'r12']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r9', 'rTransit', 'r13', 'rTransit', 'r10', 'rTransit', 'r2', 'r4', 'r2', 'rTransit', 'r8']</t>
+          <t>['None', 'None', 'None', 'r7', 'r7', 'rTransit', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r7', 'r2', 'rTransit', 'r9', 'r8']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>['rTransit', 'r5', 'r4', 'rTransit', 'r10', 'rTransit', 'r4', 'r4', 'rTransit', 'rTransit', 'r11', 'rTransit', 'r8', 'rTransit', 'r11']</t>
+          <t>['r1', 'rTransit', 'r12', 'r10', 'rTransit', 'r13', 'r13', 'rTransit', 'r9', 'rTransit', 'r13', 'rTransit', 'r9', 'rTransit', 'r13']</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['r11', 'rTransit', 'rTransit', 'r7', 'rTransit', 'r5', 'rTransit', 'r10', 'rTransit', 'r3', 'rTransit', 'r9', 'rTransit', 'r2', 'r7']</t>
+          <t>['r11', 'rTransit', 'r10', 'rTransit', 'r8', 'rTransit', 'r3', 'rTransit', 'r12', 'rTransit', 'r4', 'r5', 'r4', 'rTransit', 'r8']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'rTransit', 'r11', 'rTransit', 'r8', 'r5', 'rTransit', 'r10', 'rTransit', 'r3', 'rTransit', 'r10']</t>
+          <t>['None', 'None', 'None', 'r2', 'r7', 'rTransit', 'r12', 'rTransit', 'r4', 'rTransit', 'rTransit', 'r11', 'r11', 'r13', 'r13']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>['rTransit', 'r9', 'r9', 'rTransit', 'r12', 'r12', 'rTransit', 'r3', 'rTransit', 'r12', 'r12', 'rTransit', 'r9', 'rTransit', 'r3']</t>
+          <t>['rTransit', 'r10', 'rTransit', 'r1', 'r2', 'rTransit', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r5', 'rTransit', 'r10', 'rTransit', 'r11']</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r2', 'r4', 'rTransit', 'r12', 'rTransit', 'r9', 'rTransit', 'r4', 'rTransit', 'r12', 'rTransit', 'r7', 'r7']</t>
+          <t>['rTransit', 'rTransit', 'r3', 'rTransit', 'r7', 'r2', 'rTransit', 'r12', 'rTransit', 'r9', 'rTransit', 'r11', 'rTransit', 'r3', 'r3']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r10', 'rTransit', 'r11', 'rTransit', 'r9', 'rTransit', 'r5', 'r4', 'rTransit', 'r10', 'r9']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'rTransit', 'r13', 'rTransit', 'r12', 'rTransit', 'r2', 'rTransit', 'r5', 'rTransit', 'r10', 'r10']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r4', 'r4', 'rTransit', 'rTransit', 'r13', 'rTransit', 'r12', 'rTransit', 'r9', 'r8']</t>
+          <t>['r2', 'rTransit', 'r9', 'rTransit', 'r3', 'rTransit', 'r9', 'rTransit', 'r5', 'rTransit', 'r7', 'rTransit', 'r12', 'rTransit', 'r9']</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['rTransit', 'r8', 'rTransit', 'r11', 'rTransit', 'r10', 'rTransit', 'r7', 'rTransit', 'r12', 'rTransit', 'r9', 'rTransit', 'r4', 'r7']</t>
+          <t>['rTransit', 'rTransit', 'r5', 'rTransit', 'r10', 'r10', 'rTransit', 'r5', 'r5', 'r8', 'rTransit', 'r3', 'rTransit', 'r11', 'r11']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r12', 'rTransit', 'r8', 'rTransit', 'r3', 'r4', 'r4', 'r5', 'r3', 'r2', 'r3']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r5', 'r3', 'rTransit', 'r11', 'r12', 'r12', 'rTransit', 'r8', 'rTransit', 'r3', 'r5']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>['r4', 'rTransit', 'r12', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r2', 'rTransit', 'r9', 'r10', 'r9']</t>
+          <t>['r7', 'rTransit', 'r5', 'r5', 'r4', 'r3', 'rTransit', 'r8', 'r5', 'rTransit', 'r12', 'rTransit', 'r7', 'r2', 'r3']</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r2', 'r4', 'rTransit', 'r12', 'r11', 'rTransit', 'r3']</t>
+          <t>['rTransit', 'rTransit', 'r4', 'r4', 'rTransit', 'rTransit', 'r13', 'r13', 'r11', 'rTransit', 'r9', 'r8', 'rTransit', 'r13', 'r11']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'r7', 'rTransit', 'r5', 'rTransit', 'r9', 'rTransit', 'r12', 'r12', 'r12', 'rTransit', 'r8', 'r9']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r9', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r11', 'rTransit', 'rTransit', 'r7', 'r4', 'r3']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>['r4', 'r5', 'rTransit', 'r10', 'rTransit', 'r3', 'rTransit', 'r7', 'r4', 'rTransit', 'r8', 'r9', 'r8', 'rTransit', 'r4']</t>
+          <t>['rTransit', 'r5', 'r5', 'rTransit', 'r7', 'rTransit', 'r8', 'rTransit', 'r3', 'r3', 'rTransit', 'r12', 'rTransit', 'r7', 'r7']</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['r13', 'rTransit', 'r10', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r2', 'rTransit', 'r12', 'r10', 'r10', 'r12', 'rTransit', 'r5']</t>
+          <t>['rTransit', 'rTransit', 'r4', 'r1', 'r3', 'r5', 'rTransit', 'r9', 'rTransit', 'r3', 'r3', 'r4', 'rTransit', 'rTransit', 'r13']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'rTransit', 'r11', 'r11', 'r12', 'r12', 'r10', 'r10', 'rTransit', 'r5', 'rTransit', 'r2']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r12', 'r12', 'rTransit', 'r8', 'rTransit', 'r12', 'r12', 'rTransit', 'r9', 'rTransit', 'r4']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>['r1', 'rTransit', 'r12', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r11', 'rTransit', 'r8', 'rTransit', 'r13', 'rTransit', 'rTransit', 'r3']</t>
+          <t>['rTransit', 'r12', 'rTransit', 'r3', 'rTransit', 'r11', 'r12', 'rTransit', 'r2', 'rTransit', 'r5', 'r5', 'rTransit', 'r9', 'r10']</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['rTransit', 'rTransit', 'r7', 'r2', 'rTransit', 'r8', 'rTransit', 'r10', 'rTransit', 'r13', 'rTransit', 'r9', 'rTransit', 'r4', 'r4']</t>
+          <t>['rTransit', 'rTransit', 'r3', 'rTransit', 'r11', 'rTransit', 'r10', 'rTransit', 'r11', 'rTransit', 'r8', 'rTransit', 'r12', 'rTransit', 'r5']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['None', 'None', 'None', 'rTransit', 'r8', 'rTransit', 'r13', 'rTransit', 'r9', 'r10', 'rTransit', 'r2', 'rTransit', 'rTransit', 'r13']</t>
+          <t>['None', 'None', 'None', 'rTransit', 'r10', 'rTransit', 'r11', 'r12', 'rTransit', 'r4', 'rTransit', 'rTransit', 'r11', 'rTransit', 'r5']</t>
         </is>
       </c>
     </row>

</xml_diff>